<commit_message>
Forget password remove and & new data sheet
</commit_message>
<xml_diff>
--- a/storage/app/data/MasterTables.xlsx
+++ b/storage/app/data/MasterTables.xlsx
@@ -5151,7 +5151,7 @@
     <t>08/07/2021</t>
   </si>
   <si>
-    <t>08/07/2022</t>
+    <t>09/06/2022</t>
   </si>
   <si>
     <t>Melody Byrne</t>
@@ -6384,10 +6384,10 @@
     <t>12/09/2016</t>
   </si>
   <si>
-    <t>09/06/2021</t>
-  </si>
-  <si>
-    <t>06/06/2022</t>
+    <t>07/06/2022</t>
+  </si>
+  <si>
+    <t>07/06/2023</t>
   </si>
   <si>
     <t>90</t>
@@ -78146,7 +78146,7 @@
       </c>
       <c r="F90" s="20">
         <f t="shared" si="10"/>
-        <v>36255.91</v>
+        <v>32279.11</v>
       </c>
       <c r="G90" s="21"/>
       <c r="H90" s="21"/>
@@ -78167,7 +78167,7 @@
         <v>1485.75</v>
       </c>
       <c r="U90" s="21">
-        <v>21241.91</v>
+        <v>17265.11</v>
       </c>
     </row>
     <row r="91">
@@ -79754,12 +79754,12 @@
       </c>
       <c r="F130" s="20">
         <f t="shared" si="16"/>
-        <v>13613.13</v>
+        <v>27088.04</v>
       </c>
       <c r="G130" s="21"/>
       <c r="H130" s="21"/>
       <c r="I130" s="21">
-        <v>100.0</v>
+        <v>199.73</v>
       </c>
       <c r="J130" s="21"/>
       <c r="K130" s="21"/>
@@ -79772,10 +79772,10 @@
       <c r="R130" s="21"/>
       <c r="S130" s="21"/>
       <c r="T130" s="21">
-        <v>1485.75</v>
+        <v>2866.41</v>
       </c>
       <c r="U130" s="21">
-        <v>12027.38</v>
+        <v>24021.9</v>
       </c>
     </row>
     <row r="131">
@@ -80772,7 +80772,7 @@
         <v>2637</v>
       </c>
       <c r="F154" s="20">
-        <f t="shared" ref="F154:F163" si="17">SUM(G154:U154)</f>
+        <f t="shared" ref="F154:F164" si="17">SUM(G154:U154)</f>
         <v>17586.92</v>
       </c>
       <c r="G154" s="21"/>
@@ -81188,7 +81188,8 @@
         <v>2714</v>
       </c>
       <c r="F164" s="20">
-        <v>3513.13</v>
+        <f t="shared" si="17"/>
+        <v>13513.13</v>
       </c>
       <c r="G164" s="21"/>
       <c r="H164" s="21"/>
@@ -81206,7 +81207,9 @@
       <c r="T164" s="21">
         <v>1485.75</v>
       </c>
-      <c r="U164" s="21"/>
+      <c r="U164" s="21">
+        <v>12027.38</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>